<commit_message>
Update v0.22 (Add Agoraphobia section)
</commit_message>
<xml_diff>
--- a/episodes_course.xlsx
+++ b/episodes_course.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike.xiao/Documents/GitHub/KSADS_ML_Applet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185EF6C0-BF75-344F-9EB8-31C8B2B3DA4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB8F46C-37E3-C74B-A086-ADADF0FFA4BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15740" xr2:uid="{E7DDDB91-5224-7549-BE4C-FBC1264312E8}"/>
+    <workbookView xWindow="1860" yWindow="1300" windowWidth="27240" windowHeight="15740" activeTab="1" xr2:uid="{E7DDDB91-5224-7549-BE4C-FBC1264312E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
   <si>
     <t>Episodes: Onset</t>
   </si>
@@ -138,6 +139,102 @@
   </si>
   <si>
     <t xml:space="preserve">0, 0 | 1, 1 | 2, 2 | 3, 3 | 4, 4 | 5, 5 | 6, 6 | 7, 7 | 8, 8 | 9, 9 | 10, 10 | 998, Unknown </t>
+  </si>
+  <si>
+    <t>Help-Seeking Treatment (Lifetime)</t>
+  </si>
+  <si>
+    <t>descriptive</t>
+  </si>
+  <si>
+    <t>What kind of person/people did you get help from? \r\n\r\n _INTERVIEWER: Refer to Participant Card 13 (Professional/Treatment), record and code responses on the following screens._</t>
+  </si>
+  <si>
+    <t>dontKnow</t>
+  </si>
+  <si>
+    <t>Specify (Professional/Treatment 1):</t>
+  </si>
+  <si>
+    <t>Code (Professional/Treatment 1):</t>
+  </si>
+  <si>
+    <t>Specify (Professional/Treatment 2):</t>
+  </si>
+  <si>
+    <t>Code (Professional/Treatment 2):</t>
+  </si>
+  <si>
+    <t>Specify (Professional/Treatment 3):</t>
+  </si>
+  <si>
+    <t>Code (Professional/Treatment 3):</t>
+  </si>
+  <si>
+    <t>_INTERVIEWER: If you listed multiple people, ask this question. If not, **Skip**:_ \r\n\r\n Who did you get help from the first time? \r\n\r\n Specify (Professional/Treatment):</t>
+  </si>
+  <si>
+    <t>Code (Professional/Treatment):</t>
+  </si>
+  <si>
+    <t>How old were you the first time you got help?</t>
+  </si>
+  <si>
+    <t>Are you getting help now?</t>
+  </si>
+  <si>
+    <t>If no, how old were you the last time you got help?</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>What did the professional say that you had (diagnoses given)? List:</t>
+  </si>
+  <si>
+    <t>checkbox</t>
+  </si>
+  <si>
+    <t>What kind of treatment(s) have you gotten? _(Check all that apply)_</t>
+  </si>
+  <si>
+    <t>1, Out-patient (Going to see someone in an office) | 2, In-patient (Staying in a hospital) | 3, Other</t>
+  </si>
+  <si>
+    <t>Were you on medications? \r\n\r\n _INTERVIEWER: Refer to Participant Card 9 (Medications), record and code responses in the following screens._</t>
+  </si>
+  <si>
+    <t>Specify (Medication 1):</t>
+  </si>
+  <si>
+    <t>Code (Medication 1):</t>
+  </si>
+  <si>
+    <t>Specify (Medication 2):</t>
+  </si>
+  <si>
+    <t>Code (Medication 2):</t>
+  </si>
+  <si>
+    <t>Specify (Medication 3):</t>
+  </si>
+  <si>
+    <t>Code (Medication 3):</t>
+  </si>
+  <si>
+    <t>Specify (Medication 4):</t>
+  </si>
+  <si>
+    <t>Code (Medication 4):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Did anyone, like a teacher or family member, suggest that you get help for these symptoms? </t>
+  </si>
+  <si>
+    <t>Did you ever go to see a doctor, nurse, psychologist, social worker, school counselor, minister/priest or other professional to get help for list symptoms?</t>
+  </si>
+  <si>
+    <t>Specify (Other treatment):</t>
   </si>
 </sst>
 </file>
@@ -173,11 +270,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,7 +592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5935D68C-F5D5-7B41-8A61-1FDAB6BFC28C}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -688,12 +786,397 @@
       <c r="A12" t="s">
         <v>33</v>
       </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F12" t="s">
         <v>34</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88CD9B3-EBF6-A64F-A63A-5E7603F9F99D}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="92.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update v0.23 (Add OCD section)
</commit_message>
<xml_diff>
--- a/episodes_course.xlsx
+++ b/episodes_course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike.xiao/Documents/GitHub/KSADS_ML_Applet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB8F46C-37E3-C74B-A086-ADADF0FFA4BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9C155B-A4CC-F343-B17B-FA325CEC9A9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1300" windowWidth="27240" windowHeight="15740" activeTab="1" xr2:uid="{E7DDDB91-5224-7549-BE4C-FBC1264312E8}"/>
+    <workbookView xWindow="440" yWindow="1300" windowWidth="27240" windowHeight="15740" activeTab="1" xr2:uid="{E7DDDB91-5224-7549-BE4C-FBC1264312E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,15 +60,9 @@
     <t>Episodes: Current</t>
   </si>
   <si>
-    <t>Are you still having these behaviors/feelings **now**?</t>
-  </si>
-  <si>
     <t>Episodes: Most Recent</t>
   </si>
   <si>
-    <t>How old were you the **last time** you had these behaviors/feelings?</t>
-  </si>
-  <si>
     <t>AGE</t>
   </si>
   <si>
@@ -129,9 +123,6 @@
     <t>How old were you then?</t>
   </si>
   <si>
-    <t>How old were you the **first time** you had these behaviors/feelings? (record age or "always")</t>
-  </si>
-  <si>
     <t>Please look at Participant Card 8: Distress/Impairment. \r\n\r\n _INTERVIEWER: Remind child how to use scale, if necessary._</t>
   </si>
   <si>
@@ -198,9 +189,6 @@
     <t>What kind of treatment(s) have you gotten? _(Check all that apply)_</t>
   </si>
   <si>
-    <t>1, Out-patient (Going to see someone in an office) | 2, In-patient (Staying in a hospital) | 3, Other</t>
-  </si>
-  <si>
     <t>Were you on medications? \r\n\r\n _INTERVIEWER: Refer to Participant Card 9 (Medications), record and code responses in the following screens._</t>
   </si>
   <si>
@@ -231,10 +219,22 @@
     <t xml:space="preserve">Did anyone, like a teacher or family member, suggest that you get help for these symptoms? </t>
   </si>
   <si>
-    <t>Did you ever go to see a doctor, nurse, psychologist, social worker, school counselor, minister/priest or other professional to get help for list symptoms?</t>
+    <t>Did you ever go to see a doctor, nurse, psychologist, social worker, school counselor, minister/priest or other professional to get help for (list symptoms)?</t>
   </si>
   <si>
     <t>Specify (Other treatment):</t>
+  </si>
+  <si>
+    <t>Are you still having these fears **now**?</t>
+  </si>
+  <si>
+    <t>How old were you the **first time** you had these fears? (record age or "always")</t>
+  </si>
+  <si>
+    <t>How old were you the **last time** you had these fears?</t>
+  </si>
+  <si>
+    <t>1, Out-patient (Going to see someone in an office) | 2, In-patient (Staying in a hospital) | 3, Self Help | 4, Other</t>
   </si>
 </sst>
 </file>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5935D68C-F5D5-7B41-8A61-1FDAB6BFC28C}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -614,7 +614,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="M1" t="s">
         <v>6</v>
@@ -631,7 +631,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
@@ -642,41 +642,41 @@
     </row>
     <row r="3" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="M3" t="s">
         <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -685,32 +685,32 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
       </c>
       <c r="M5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -719,30 +719,30 @@
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
         <v>3</v>
       </c>
       <c r="M7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="H8" t="s">
         <v>23</v>
-      </c>
-      <c r="G8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" t="s">
-        <v>25</v>
       </c>
       <c r="M8" t="s">
         <v>4</v>
@@ -750,50 +750,50 @@
     </row>
     <row r="9" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" t="s">
         <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
         <v>33</v>
       </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88CD9B3-EBF6-A64F-A63A-5E7603F9F99D}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -818,7 +818,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -828,7 +828,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -844,7 +844,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>3</v>
@@ -855,94 +855,94 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -954,7 +954,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -966,7 +966,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -978,7 +978,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -992,7 +992,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>3</v>
@@ -1006,7 +1006,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -1015,10 +1015,10 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -1029,13 +1029,13 @@
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1043,10 +1043,10 @@
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -1060,7 +1060,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>3</v>
@@ -1069,112 +1069,112 @@
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F26" s="2"/>
     </row>

</xml_diff>

<commit_message>
Update v0.24 (Add ADHD section, modify age questions)
Add: \r\n\r\n _Code 998 if "always", 999 if "unknown"._ at the end of each question asking for age
</commit_message>
<xml_diff>
--- a/episodes_course.xlsx
+++ b/episodes_course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike.xiao/Documents/GitHub/KSADS_ML_Applet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9C155B-A4CC-F343-B17B-FA325CEC9A9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF22D7F-498A-5342-97D8-31CC24218394}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="1300" windowWidth="27240" windowHeight="15740" activeTab="1" xr2:uid="{E7DDDB91-5224-7549-BE4C-FBC1264312E8}"/>
+    <workbookView xWindow="660" yWindow="940" windowWidth="27240" windowHeight="15740" xr2:uid="{E7DDDB91-5224-7549-BE4C-FBC1264312E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="68">
   <si>
     <t>Episodes: Onset</t>
   </si>
@@ -135,6 +135,9 @@
     <t>Help-Seeking Treatment (Lifetime)</t>
   </si>
   <si>
+    <t>Did you ever go to see a doctor, nurse, psychologist, social worker, school counselor, minister/priest or other professional to get help for (list behaviors/feelings)?</t>
+  </si>
+  <si>
     <t>descriptive</t>
   </si>
   <si>
@@ -216,25 +219,25 @@
     <t>Code (Medication 4):</t>
   </si>
   <si>
-    <t xml:space="preserve">Did anyone, like a teacher or family member, suggest that you get help for these symptoms? </t>
-  </si>
-  <si>
-    <t>Did you ever go to see a doctor, nurse, psychologist, social worker, school counselor, minister/priest or other professional to get help for (list symptoms)?</t>
-  </si>
-  <si>
     <t>Specify (Other treatment):</t>
   </si>
   <si>
     <t>Are you still having these fears **now**?</t>
   </si>
   <si>
-    <t>How old were you the **first time** you had these fears? (record age or "always")</t>
-  </si>
-  <si>
     <t>How old were you the **last time** you had these fears?</t>
   </si>
   <si>
-    <t>1, Out-patient (Going to see someone in an office) | 2, In-patient (Staying in a hospital) | 3, Self Help | 4, Other</t>
+    <t xml:space="preserve">Did anyone, like a teacher or family member, suggest that you get help for these (list behaviors/feelings)? </t>
+  </si>
+  <si>
+    <t>Were you placed in special classes at school because of your (list symptoms)?</t>
+  </si>
+  <si>
+    <t>1, Out-patient (Going to see someone in an office) | 2, In-patient (Staying in a hospital) | 3, Special classes at school (IEP etc) | 4, Other</t>
+  </si>
+  <si>
+    <t>How old were you the **first time** you had these fears? \r\n\r\n _Code 998 if "always", 999 if "unknown"._</t>
   </si>
 </sst>
 </file>
@@ -592,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5935D68C-F5D5-7B41-8A61-1FDAB6BFC28C}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E2:E3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -614,7 +617,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="M1" t="s">
         <v>6</v>
@@ -631,7 +634,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
@@ -648,7 +651,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -787,7 +790,7 @@
         <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>29</v>
@@ -803,10 +806,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88CD9B3-EBF6-A64F-A63A-5E7603F9F99D}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -828,13 +831,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -844,7 +847,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>3</v>
@@ -852,34 +855,36 @@
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
@@ -893,7 +898,7 @@
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
@@ -907,7 +912,7 @@
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
@@ -921,7 +926,7 @@
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
@@ -935,7 +940,7 @@
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
@@ -946,9 +951,11 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
         <v>5</v>
@@ -958,7 +965,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -984,106 +991,104 @@
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
       <c r="D17" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
-      <c r="B18" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
@@ -1097,7 +1102,7 @@
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
@@ -1111,7 +1116,7 @@
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
@@ -1125,7 +1130,7 @@
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
@@ -1139,7 +1144,7 @@
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
@@ -1153,7 +1158,7 @@
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
@@ -1167,7 +1172,7 @@
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
@@ -1177,6 +1182,20 @@
         <v>59</v>
       </c>
       <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update v0.25 (add ODD and Conduct Disorder Sections)
</commit_message>
<xml_diff>
--- a/episodes_course.xlsx
+++ b/episodes_course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike.xiao/Documents/GitHub/KSADS_ML_Applet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF22D7F-498A-5342-97D8-31CC24218394}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945EF9E1-FC41-6A41-A9DB-6A467B4E5983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="940" windowWidth="27240" windowHeight="15740" xr2:uid="{E7DDDB91-5224-7549-BE4C-FBC1264312E8}"/>
+    <workbookView xWindow="660" yWindow="940" windowWidth="27240" windowHeight="15740" activeTab="1" xr2:uid="{E7DDDB91-5224-7549-BE4C-FBC1264312E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="69">
   <si>
     <t>Episodes: Onset</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Help-Seeking Treatment (Lifetime)</t>
   </si>
   <si>
-    <t>Did you ever go to see a doctor, nurse, psychologist, social worker, school counselor, minister/priest or other professional to get help for (list behaviors/feelings)?</t>
-  </si>
-  <si>
     <t>descriptive</t>
   </si>
   <si>
@@ -171,15 +168,9 @@
     <t>Code (Professional/Treatment):</t>
   </si>
   <si>
-    <t>How old were you the first time you got help?</t>
-  </si>
-  <si>
     <t>Are you getting help now?</t>
   </si>
   <si>
-    <t>If no, how old were you the last time you got help?</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -192,6 +183,9 @@
     <t>What kind of treatment(s) have you gotten? _(Check all that apply)_</t>
   </si>
   <si>
+    <t>1, Out-patient (Going to see someone in an office) | 2, In-patient (Staying in a hospital) | 3, Other</t>
+  </si>
+  <si>
     <t>Were you on medications? \r\n\r\n _INTERVIEWER: Refer to Participant Card 9 (Medications), record and code responses in the following screens._</t>
   </si>
   <si>
@@ -225,19 +219,28 @@
     <t>Are you still having these fears **now**?</t>
   </si>
   <si>
-    <t>How old were you the **last time** you had these fears?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Did anyone, like a teacher or family member, suggest that you get help for these (list behaviors/feelings)? </t>
-  </si>
-  <si>
-    <t>Were you placed in special classes at school because of your (list symptoms)?</t>
-  </si>
-  <si>
-    <t>1, Out-patient (Going to see someone in an office) | 2, In-patient (Staying in a hospital) | 3, Special classes at school (IEP etc) | 4, Other</t>
-  </si>
-  <si>
     <t>How old were you the **first time** you had these fears? \r\n\r\n _Code 998 if "always", 999 if "unknown"._</t>
+  </si>
+  <si>
+    <t>Did you ever go to see a doctor, nurse, psychologist, social worker, school counselor, minister/priest or other professional to get help for (list behaviors)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Did anyone, like a teacher or family member, suggest that you get help for these behaviors? </t>
+  </si>
+  <si>
+    <t>How old were you the **last time** you had these fears? \r\n\r\n _Code 998 if "always", 999 if "unknown"._</t>
+  </si>
+  <si>
+    <t>Did a judge or probation officer ever require you to obtain treatment?</t>
+  </si>
+  <si>
+    <t>Were you placed in special classes at school because of your (list behaviors)?</t>
+  </si>
+  <si>
+    <t>How old were you the first time you got help? \r\n\r\n _Code 998 if "always", 999 if "unknown"._</t>
+  </si>
+  <si>
+    <t>If no, how old were you the last time you got help? \r\n\r\n _Code 998 if "always", 999 if "unknown"._</t>
   </si>
 </sst>
 </file>
@@ -595,7 +598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5935D68C-F5D5-7B41-8A61-1FDAB6BFC28C}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -617,7 +620,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="M1" t="s">
         <v>6</v>
@@ -634,7 +637,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
@@ -651,7 +654,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -790,7 +793,7 @@
         <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>29</v>
@@ -806,10 +809,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88CD9B3-EBF6-A64F-A63A-5E7603F9F99D}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -831,7 +834,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -847,13 +850,13 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -863,7 +866,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>3</v>
@@ -871,113 +874,117 @@
     </row>
     <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -985,7 +992,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -997,205 +1004,217 @@
         <v>5</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>3</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="2">
-        <v>1</v>
-      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>66</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
       <c r="D18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F18" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
-      <c r="B19" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update v0.26 (Add eating disorder and PTSD sections, Map Variable / Field Name to @id))
"Variable / Field Name" was incorrectly mapped to skos:altLabel, while 'Identifier?' was incorrectly mapped to "@id:"
</commit_message>
<xml_diff>
--- a/episodes_course.xlsx
+++ b/episodes_course.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike.xiao/Documents/GitHub/KSADS_ML_Applet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945EF9E1-FC41-6A41-A9DB-6A467B4E5983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F48452-5D19-BF40-8190-7E0BC1448BA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="940" windowWidth="27240" windowHeight="15740" activeTab="1" xr2:uid="{E7DDDB91-5224-7549-BE4C-FBC1264312E8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
   <si>
     <t>Episodes: Onset</t>
   </si>
@@ -135,6 +135,9 @@
     <t>Help-Seeking Treatment (Lifetime)</t>
   </si>
   <si>
+    <t>Did you ever go to see a doctor, nurse, psychologist, social worker, school counselor, minister/priest or other professional to get help for (list behaviors/feelings)?</t>
+  </si>
+  <si>
     <t>descriptive</t>
   </si>
   <si>
@@ -222,25 +225,16 @@
     <t>How old were you the **first time** you had these fears? \r\n\r\n _Code 998 if "always", 999 if "unknown"._</t>
   </si>
   <si>
-    <t>Did you ever go to see a doctor, nurse, psychologist, social worker, school counselor, minister/priest or other professional to get help for (list behaviors)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Did anyone, like a teacher or family member, suggest that you get help for these behaviors? </t>
-  </si>
-  <si>
     <t>How old were you the **last time** you had these fears? \r\n\r\n _Code 998 if "always", 999 if "unknown"._</t>
   </si>
   <si>
-    <t>Did a judge or probation officer ever require you to obtain treatment?</t>
-  </si>
-  <si>
-    <t>Were you placed in special classes at school because of your (list behaviors)?</t>
-  </si>
-  <si>
     <t>How old were you the first time you got help? \r\n\r\n _Code 998 if "always", 999 if "unknown"._</t>
   </si>
   <si>
     <t>If no, how old were you the last time you got help? \r\n\r\n _Code 998 if "always", 999 if "unknown"._</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Did anyone, like a teacher or family member, suggest that you get help for (list behaviors/feelings)? </t>
   </si>
 </sst>
 </file>
@@ -599,7 +593,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,7 +614,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M1" t="s">
         <v>6</v>
@@ -637,7 +631,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
@@ -654,7 +648,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -793,7 +787,7 @@
         <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>29</v>
@@ -809,10 +803,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88CD9B3-EBF6-A64F-A63A-5E7603F9F99D}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,13 +828,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -850,141 +844,133 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -992,21 +978,25 @@
         <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
@@ -1016,205 +1006,177 @@
         <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
-      <c r="B15" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>3</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
       <c r="D16" s="2" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2">
+      <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>3</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update v0.27 (clean up new sections for mistakes)
</commit_message>
<xml_diff>
--- a/episodes_course.xlsx
+++ b/episodes_course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike.xiao/Documents/GitHub/KSADS_ML_Applet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F48452-5D19-BF40-8190-7E0BC1448BA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52913EA-0E98-B742-B47B-DBF667630443}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="940" windowWidth="27240" windowHeight="15740" activeTab="1" xr2:uid="{E7DDDB91-5224-7549-BE4C-FBC1264312E8}"/>
+    <workbookView xWindow="1360" yWindow="620" windowWidth="27240" windowHeight="15740" activeTab="1" xr2:uid="{E7DDDB91-5224-7549-BE4C-FBC1264312E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="67">
   <si>
     <t>Episodes: Onset</t>
   </si>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88CD9B3-EBF6-A64F-A63A-5E7603F9F99D}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,7 +948,9 @@
     </row>
     <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
         <v>5</v>
@@ -960,7 +962,9 @@
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
update v0.28 (add alcohol abuse and tobaco sections)
</commit_message>
<xml_diff>
--- a/episodes_course.xlsx
+++ b/episodes_course.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike.xiao/Documents/GitHub/KSADS_ML_Applet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52913EA-0E98-B742-B47B-DBF667630443}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED5DE45-FB0D-1540-8BA5-6C691069C5A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="620" windowWidth="27240" windowHeight="15740" activeTab="1" xr2:uid="{E7DDDB91-5224-7549-BE4C-FBC1264312E8}"/>
+    <workbookView xWindow="14260" yWindow="480" windowWidth="15260" windowHeight="16740" activeTab="1" xr2:uid="{E7DDDB91-5224-7549-BE4C-FBC1264312E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="83">
   <si>
     <t>Episodes: Onset</t>
   </si>
@@ -177,18 +178,12 @@
     <t>notes</t>
   </si>
   <si>
-    <t>What did the professional say that you had (diagnoses given)? List:</t>
-  </si>
-  <si>
     <t>checkbox</t>
   </si>
   <si>
     <t>What kind of treatment(s) have you gotten? _(Check all that apply)_</t>
   </si>
   <si>
-    <t>1, Out-patient (Going to see someone in an office) | 2, In-patient (Staying in a hospital) | 3, Other</t>
-  </si>
-  <si>
     <t>Were you on medications? \r\n\r\n _INTERVIEWER: Refer to Participant Card 9 (Medications), record and code responses in the following screens._</t>
   </si>
   <si>
@@ -235,6 +230,60 @@
   </si>
   <si>
     <t xml:space="preserve">Did anyone, like a teacher or family member, suggest that you get help for (list behaviors/feelings)? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What did the professional(s) (doctors) say was the problem? (diagnoses given)? List:     </t>
+  </si>
+  <si>
+    <t>1, Out-patient (Going to an office to see someone or participating in group treatment not in a hospital)| 2, In-patient (Residential/hospital) | 3, Other</t>
+  </si>
+  <si>
+    <t>dcalc011 &gt; 3</t>
+  </si>
+  <si>
+    <t>[dcalc018] &lt; 4</t>
+  </si>
+  <si>
+    <t>[dcalc022] &lt; 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[dcalc025] = 0 </t>
+  </si>
+  <si>
+    <t>[dcalc027] = 0</t>
+  </si>
+  <si>
+    <t>[dcalc028] = 0</t>
+  </si>
+  <si>
+    <t>[dcalc029] = 0</t>
+  </si>
+  <si>
+    <t>[dcalc030] = 0</t>
+  </si>
+  <si>
+    <t>[dcalc031] = 0</t>
+  </si>
+  <si>
+    <t>[dcalc032] = 0</t>
+  </si>
+  <si>
+    <t>[dcalc034] = 0</t>
+  </si>
+  <si>
+    <t>[dcalc036] = 0</t>
+  </si>
+  <si>
+    <t>[dcalc038] = 0</t>
+  </si>
+  <si>
+    <t>[dcalc040] = 0</t>
+  </si>
+  <si>
+    <t>[dcalc043] = 0</t>
+  </si>
+  <si>
+    <t>[dcalc047] = 0</t>
   </si>
 </sst>
 </file>
@@ -614,7 +663,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M1" t="s">
         <v>6</v>
@@ -631,7 +680,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
@@ -648,7 +697,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -803,10 +852,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88CD9B3-EBF6-A64F-A63A-5E7603F9F99D}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -828,7 +877,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -982,7 +1031,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -1010,7 +1059,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -1019,10 +1068,10 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -1033,13 +1082,13 @@
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F16" s="2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1050,7 +1099,7 @@
         <v>46</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -1064,7 +1113,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>3</v>
@@ -1080,7 +1129,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -1094,7 +1143,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F20" s="2"/>
     </row>
@@ -1108,7 +1157,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -1122,7 +1171,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -1136,7 +1185,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F23" s="2"/>
     </row>
@@ -1150,7 +1199,7 @@
         <v>5</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F24" s="2"/>
     </row>
@@ -1164,7 +1213,7 @@
         <v>5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F25" s="2"/>
     </row>
@@ -1178,9 +1227,115 @@
         <v>5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F26" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D28" s="1"/>
+      <c r="E28"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D29" s="1"/>
+      <c r="E29"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6D9769-36FF-804A-A1F1-3A9B87C4446F}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>